<commit_message>
data into phyloseq, low read samples trimmed and NTC evaluated
</commit_message>
<xml_diff>
--- a/MCL_SymPortal_submission_input.xlsx
+++ b/MCL_SymPortal_submission_input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shayle/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shayle/Desktop/Microbial landscape/ITS2_Summer_symportal2020/Microbial_landscape_MCL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41DAF975-EA17-784B-9CA4-050EF33B8CA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B760C7-DEB6-BB4F-A95E-395B31F6F663}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34980" yWindow="560" windowWidth="25980" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3981" uniqueCount="1230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3979" uniqueCount="1230">
   <si>
     <t>sample_name</t>
   </si>
@@ -4080,8 +4080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N386"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4149,12 +4149,6 @@
       </c>
       <c r="L2" t="s">
         <v>72</v>
-      </c>
-      <c r="M2" t="s">
-        <v>73</v>
-      </c>
-      <c r="N2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>